<commit_message>
vault backup: 2025-10-17 16:48:16
</commit_message>
<xml_diff>
--- a/Wizarding World/World/Potions/W&W Potion Spreadsheet.xlsx
+++ b/Wizarding World/World/Potions/W&W Potion Spreadsheet.xlsx
@@ -7,7 +7,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28843E48-FCD1-4B53-9D1C-82FCBFBE3B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87376CA-C0F2-4336-A9AD-25A95F70466E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -18,8 +18,8 @@
     <sheet name="Ingred. Prices" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="false">'Potion Grid'!$A$1:$BT$211</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="false">Ingredients!$A$1:$E$232</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="false">'Potion Grid'!$A$1:$BT$211</definedName>
     <definedName name="_xlnm._FilterDatabase" hidden="false">Potions!$A$1:$M$1038</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2081,11 +2081,21 @@
     </font>
     <font>
       <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="9.00"/>
       <family val="2"/>
     </font>
     <font>
       <name val="Arial"/>
+      <sz val="10.00"/>
       <color rgb="FF000000"/>
       <family val="2"/>
     </font>
@@ -2096,17 +2106,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <sz val="10.00"/>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <b/>
-      <family val="2"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2119,13 +2119,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2143,6 +2179,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2155,67 +2209,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFF3F3F3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2306,170 +2306,170 @@
     <xf fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="0"/>
     </xf>
-    <xf fontId="2" applyFont="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf fontId="1" applyFont="1" borderId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" applyFont="1" fillId="3" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" applyFont="1" borderId="4" applyBorder="1"/>
-    <xf fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
-    </xf>
-    <xf fontId="1" applyFont="1"/>
-    <xf fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
+    <xf fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="3" applyFont="1" fillId="7" applyFill="1" borderId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
+      <alignment wrapText="0"/>
     </xf>
     <xf fontId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
+    <xf fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
     <xf fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
+    <xf fontId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" applyFont="1"/>
+    <xf fontId="6" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="0"/>
+    </xf>
+    <xf fontId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf fontId="1" applyFont="1" borderId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" applyFont="1" borderId="4" applyBorder="1"/>
+    <xf fontId="7" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="1" applyFont="1" fillId="10" applyFill="1" borderId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
+    <xf fontId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="0"/>
+    </xf>
+    <xf fontId="1" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" applyFont="1" fillId="14" applyFill="1" borderId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="0"/>
     </xf>
     <xf fontId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="0"/>
-    </xf>
-    <xf fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
-      <alignment wrapText="0"/>
-    </xf>
-    <xf fontId="1" applyFont="1" fillId="11" applyFill="1" borderId="7" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" applyFont="1" fillId="15" applyFill="1" borderId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf fontId="3" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="1" applyFont="1" fillId="13" applyFill="1" borderId="8" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="4" applyFont="1" applyAlignment="1">
+    <xf fontId="6" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="0"/>
     </xf>
-    <xf fontId="6" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="3" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="1" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
+    <xf fontId="1" applyFont="1" fillId="18" applyFill="1" borderId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="3" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="4" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="0"/>
-    </xf>
-    <xf fontId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf xfId="25" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
+    <xf xfId="20" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="7" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1"/>
-    <xf xfId="15" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
+    <xf xfId="12" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1"/>
+    <xf xfId="21" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf xfId="18" quotePrefix="0" pivotButton="0" fontId="5" applyFont="1" applyAlignment="1">
+    <xf xfId="10" quotePrefix="0" pivotButton="0" fontId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="0"/>
     </xf>
-    <xf xfId="29" quotePrefix="0" pivotButton="0" fontId="7" applyFont="1" applyAlignment="1">
+    <xf xfId="3" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf xfId="12" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="6" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf xfId="19" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf xfId="5" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="22" quotePrefix="0" pivotButton="0" fontId="6" applyFont="1" applyAlignment="1">
+    <xf xfId="17" quotePrefix="0" pivotButton="0" fontId="7" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="23" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
+    <xf xfId="2" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="11" quotePrefix="0" pivotButton="0" fontId="4" applyFont="1" applyAlignment="1">
+    <xf xfId="14" quotePrefix="0" pivotButton="0" fontId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf xfId="21" quotePrefix="0" pivotButton="0" fontId="4" applyFont="1" applyAlignment="1">
+    <xf xfId="13" quotePrefix="0" pivotButton="0" fontId="6" applyFont="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="0"/>
     </xf>
-    <xf xfId="28" quotePrefix="0" pivotButton="0" fontId="4" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
+    <xf xfId="28" quotePrefix="0" pivotButton="0" fontId="6" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="0"/>
     </xf>
-    <xf xfId="2" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" applyAlignment="1">
+    <xf xfId="7" quotePrefix="0" pivotButton="0" fontId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf xfId="16" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf xfId="4" quotePrefix="0" pivotButton="0" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="0"/>
     </xf>
-    <xf xfId="5" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" borderId="4" applyBorder="1"/>
-    <xf xfId="3" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" borderId="2" applyBorder="1" applyAlignment="1">
+    <xf xfId="16" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" borderId="4" applyBorder="1"/>
+    <xf xfId="15" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" borderId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="8" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
-    </xf>
-    <xf xfId="20" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="13" applyFill="1" borderId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="4" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="3" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="14" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="6" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
-    </xf>
-    <xf xfId="24" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="27" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="17" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="11" applyFill="1" borderId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="26" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="9" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="13" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="0"/>
     </xf>
     <xf xfId="1" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="0"/>
     </xf>
-    <xf xfId="10" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" fillId="7" applyFill="1" borderId="6" applyBorder="1" applyAlignment="1">
+    <xf xfId="18" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="10" applyFill="1" borderId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="29" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="18" applyFill="1" borderId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="25" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="19" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
+    <xf xfId="27" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="22" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="26" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="15" applyFill="1" borderId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="11" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="23" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="9" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
+    <xf xfId="24" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1" fillId="14" applyFill="1" borderId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="0"/>
+    </xf>
+    <xf xfId="8" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -2845,13 +2845,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="3">
-        <f ref="J2:J70" t="shared" si="14">=IF(B2="common",50,IF(B2="uncommon",250,IF(B2="rare",2500,IF(B2="very rare",25000,125000))))</f>
+        <f ref="J2:J70" t="shared" si="11">=IF(B2="common",50,IF(B2="uncommon",250,IF(B2="rare",2500,IF(B2="very rare",25000,125000))))</f>
       </c>
       <c r="K2" s="3">
-        <f ref="K2:K70" t="shared" si="15">=J2*25</f>
+        <f ref="K2:K70" t="shared" si="13">=J2*25</f>
       </c>
       <c r="L2" s="3">
-        <f ref="L2:L70" t="shared" si="11">=CONCATENATE("#### ",A2," *",C2,", ",B2,"* ",F2)</f>
+        <f ref="L2:L70" t="shared" si="14">=CONCATENATE("#### ",A2," *",C2,", ",B2,"* ",F2)</f>
       </c>
       <c r="M2" s="3">
         <f ref="M2:M70" t="shared" si="12">=CONCATENATE("___ **Recipe:** * 1 * 1 * 1 * 1 ___ **Flawed ",A2,":**",G2," ___ **Exceptional ",A2,":**",H2)</f>
@@ -2860,7 +2860,7 @@
         <v>19</v>
       </c>
       <c r="P2" s="4">
-        <f ref="P2:P6" t="shared" si="13">=COUNTIF($B:$B,O2)</f>
+        <f ref="P2:P6" t="shared" si="15">=COUNTIF($B:$B,O2)</f>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="true">
@@ -2890,13 +2890,13 @@
         <v>2</v>
       </c>
       <c r="J3" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L3" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M3" s="3">
         <f t="shared" si="12"/>
@@ -2905,7 +2905,7 @@
         <v>27</v>
       </c>
       <c r="P3" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="true">
@@ -2937,13 +2937,13 @@
         <v>2</v>
       </c>
       <c r="J4" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L4" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="12"/>
@@ -2952,7 +2952,7 @@
         <v>35</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="true">
@@ -2982,13 +2982,13 @@
         <v>2</v>
       </c>
       <c r="J5" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L5" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="12"/>
@@ -2997,7 +2997,7 @@
         <v>39</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="true">
@@ -3025,13 +3025,13 @@
         <v>2</v>
       </c>
       <c r="J6" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L6" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="12"/>
@@ -3040,7 +3040,7 @@
         <v>44</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="true">
@@ -3070,13 +3070,13 @@
         <v>2</v>
       </c>
       <c r="J7" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="12"/>
@@ -3109,13 +3109,13 @@
         <v>2</v>
       </c>
       <c r="J8" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="12"/>
@@ -3146,13 +3146,13 @@
         <v>2</v>
       </c>
       <c r="J9" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="12"/>
@@ -3185,13 +3185,13 @@
         <v>2</v>
       </c>
       <c r="J10" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L10" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="12"/>
@@ -3224,13 +3224,13 @@
         <v>2</v>
       </c>
       <c r="J11" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L11" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="12"/>
@@ -3263,13 +3263,13 @@
         <v>2</v>
       </c>
       <c r="J12" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="12"/>
@@ -3300,13 +3300,13 @@
         <v>2</v>
       </c>
       <c r="J13" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L13" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L13" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="12"/>
@@ -3339,13 +3339,13 @@
         <v>2</v>
       </c>
       <c r="J14" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L14" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L14" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="12"/>
@@ -3380,13 +3380,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L15" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L15" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="12"/>
@@ -3417,13 +3417,13 @@
         <v>2</v>
       </c>
       <c r="J16" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L16" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L16" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="12"/>
@@ -3456,13 +3456,13 @@
         <v>2</v>
       </c>
       <c r="J17" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L17" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L17" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="12"/>
@@ -3498,13 +3498,13 @@
         <v>2</v>
       </c>
       <c r="J18" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L18" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="12"/>
@@ -3535,13 +3535,13 @@
         <v>2</v>
       </c>
       <c r="J19" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L19" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L19" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="12"/>
@@ -3576,13 +3576,13 @@
         <v>2</v>
       </c>
       <c r="J20" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L20" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L20" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="12"/>
@@ -3617,13 +3617,13 @@
         <v>2</v>
       </c>
       <c r="J21" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L21" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L21" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M21" s="3">
         <f t="shared" si="12"/>
@@ -3656,13 +3656,13 @@
         <v>2</v>
       </c>
       <c r="J22" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L22" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L22" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M22" s="3">
         <f t="shared" si="12"/>
@@ -3693,13 +3693,13 @@
         <v>2</v>
       </c>
       <c r="J23" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L23" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L23" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M23" s="3">
         <f t="shared" si="12"/>
@@ -3732,13 +3732,13 @@
         <v>2</v>
       </c>
       <c r="J24" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L24" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L24" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M24" s="3">
         <f t="shared" si="12"/>
@@ -3771,13 +3771,13 @@
         <v>2</v>
       </c>
       <c r="J25" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L25" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M25" s="3">
         <f t="shared" si="12"/>
@@ -3810,13 +3810,13 @@
         <v>2</v>
       </c>
       <c r="J26" s="6">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L26" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L26" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M26" s="3">
         <f t="shared" si="12"/>
@@ -3851,13 +3851,13 @@
         <v>2</v>
       </c>
       <c r="J27" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L27" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K27" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L27" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M27" s="3">
         <f t="shared" si="12"/>
@@ -3888,13 +3888,13 @@
         <v>2</v>
       </c>
       <c r="J28" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L28" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K28" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L28" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="12"/>
@@ -3925,13 +3925,13 @@
         <v>2</v>
       </c>
       <c r="J29" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L29" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L29" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M29" s="3">
         <f t="shared" si="12"/>
@@ -3962,13 +3962,13 @@
         <v>2</v>
       </c>
       <c r="J30" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L30" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K30" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L30" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M30" s="3">
         <f t="shared" si="12"/>
@@ -4003,13 +4003,13 @@
         <v>2</v>
       </c>
       <c r="J31" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L31" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K31" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L31" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M31" s="3">
         <f t="shared" si="12"/>
@@ -4042,13 +4042,13 @@
         <v>2</v>
       </c>
       <c r="J32" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L32" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K32" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L32" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M32" s="3">
         <f t="shared" si="12"/>
@@ -4081,13 +4081,13 @@
         <v>2</v>
       </c>
       <c r="J33" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L33" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K33" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L33" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M33" s="3">
         <f t="shared" si="12"/>
@@ -4122,13 +4122,13 @@
         <v>2</v>
       </c>
       <c r="J34" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L34" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K34" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L34" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M34" s="3">
         <f t="shared" si="12"/>
@@ -4161,13 +4161,13 @@
         <v>2</v>
       </c>
       <c r="J35" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L35" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K35" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L35" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M35" s="3">
         <f t="shared" si="12"/>
@@ -4202,13 +4202,13 @@
         <v>2</v>
       </c>
       <c r="J36" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L36" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K36" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L36" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M36" s="3">
         <f t="shared" si="12"/>
@@ -4241,13 +4241,13 @@
         <v>2</v>
       </c>
       <c r="J37" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L37" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K37" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L37" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M37" s="3">
         <f t="shared" si="12"/>
@@ -4278,13 +4278,13 @@
         <v>2</v>
       </c>
       <c r="J38" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L38" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K38" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L38" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M38" s="3">
         <f t="shared" si="12"/>
@@ -4317,13 +4317,13 @@
         <v>2</v>
       </c>
       <c r="J39" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L39" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K39" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L39" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M39" s="3">
         <f t="shared" si="12"/>
@@ -4358,13 +4358,13 @@
         <v>2</v>
       </c>
       <c r="J40" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K40" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L40" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K40" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L40" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M40" s="3">
         <f t="shared" si="12"/>
@@ -4395,13 +4395,13 @@
         <v>2</v>
       </c>
       <c r="J41" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K41" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L41" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K41" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L41" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M41" s="3">
         <f t="shared" si="12"/>
@@ -4434,13 +4434,13 @@
         <v>2</v>
       </c>
       <c r="J42" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L42" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K42" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L42" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M42" s="3">
         <f t="shared" si="12"/>
@@ -4473,13 +4473,13 @@
         <v>2</v>
       </c>
       <c r="J43" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K43" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L43" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K43" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L43" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M43" s="3">
         <f t="shared" si="12"/>
@@ -4512,13 +4512,13 @@
         <v>2</v>
       </c>
       <c r="J44" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K44" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L44" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K44" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L44" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M44" s="3">
         <f t="shared" si="12"/>
@@ -4553,13 +4553,13 @@
         <v>2</v>
       </c>
       <c r="J45" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K45" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L45" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K45" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L45" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M45" s="3">
         <f t="shared" si="12"/>
@@ -4592,13 +4592,13 @@
         <v>2</v>
       </c>
       <c r="J46" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K46" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L46" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K46" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L46" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M46" s="3">
         <f t="shared" si="12"/>
@@ -4631,13 +4631,13 @@
         <v>2</v>
       </c>
       <c r="J47" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L47" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K47" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L47" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M47" s="3">
         <f t="shared" si="12"/>
@@ -4672,13 +4672,13 @@
         <v>2</v>
       </c>
       <c r="J48" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L48" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K48" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L48" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M48" s="3">
         <f t="shared" si="12"/>
@@ -4713,13 +4713,13 @@
         <v>2</v>
       </c>
       <c r="J49" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L49" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K49" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L49" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M49" s="3">
         <f t="shared" si="12"/>
@@ -4746,13 +4746,13 @@
         <v>2</v>
       </c>
       <c r="J50" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K50" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L50" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K50" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L50" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M50" s="3">
         <f t="shared" si="12"/>
@@ -4785,13 +4785,13 @@
         <v>2</v>
       </c>
       <c r="J51" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K51" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L51" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K51" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L51" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M51" s="3">
         <f t="shared" si="12"/>
@@ -4822,13 +4822,13 @@
         <v>2</v>
       </c>
       <c r="J52" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L52" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K52" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L52" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M52" s="3">
         <f t="shared" si="12"/>
@@ -4863,13 +4863,13 @@
         <v>2</v>
       </c>
       <c r="J53" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L53" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K53" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L53" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M53" s="3">
         <f t="shared" si="12"/>
@@ -4900,13 +4900,13 @@
         <v>2</v>
       </c>
       <c r="J54" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K54" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L54" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K54" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L54" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M54" s="3">
         <f t="shared" si="12"/>
@@ -4941,13 +4941,13 @@
         <v>2</v>
       </c>
       <c r="J55" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K55" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L55" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K55" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L55" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M55" s="3">
         <f t="shared" si="12"/>
@@ -4980,13 +4980,13 @@
         <v>2</v>
       </c>
       <c r="J56" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K56" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L56" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K56" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L56" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M56" s="3">
         <f t="shared" si="12"/>
@@ -5021,13 +5021,13 @@
         <v>2</v>
       </c>
       <c r="J57" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K57" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L57" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K57" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L57" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M57" s="3">
         <f t="shared" si="12"/>
@@ -5060,13 +5060,13 @@
         <v>2</v>
       </c>
       <c r="J58" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K58" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L58" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K58" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L58" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M58" s="3">
         <f t="shared" si="12"/>
@@ -5101,13 +5101,13 @@
         <v>2</v>
       </c>
       <c r="J59" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K59" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L59" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K59" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L59" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M59" s="3">
         <f t="shared" si="12"/>
@@ -5142,13 +5142,13 @@
         <v>2</v>
       </c>
       <c r="J60" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K60" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L60" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K60" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L60" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M60" s="3">
         <f t="shared" si="12"/>
@@ -5181,13 +5181,13 @@
         <v>2</v>
       </c>
       <c r="J61" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K61" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L61" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K61" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L61" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M61" s="3">
         <f t="shared" si="12"/>
@@ -5220,13 +5220,13 @@
         <v>2</v>
       </c>
       <c r="J62" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K62" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L62" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K62" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L62" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M62" s="3">
         <f t="shared" si="12"/>
@@ -5259,13 +5259,13 @@
         <v>2</v>
       </c>
       <c r="J63" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K63" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L63" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K63" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L63" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M63" s="3">
         <f t="shared" si="12"/>
@@ -5298,13 +5298,13 @@
         <v>2</v>
       </c>
       <c r="J64" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K64" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L64" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K64" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L64" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M64" s="3">
         <f t="shared" si="12"/>
@@ -5339,13 +5339,13 @@
         <v>2</v>
       </c>
       <c r="J65" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K65" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L65" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K65" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L65" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M65" s="3">
         <f t="shared" si="12"/>
@@ -5378,13 +5378,13 @@
         <v>2</v>
       </c>
       <c r="J66" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K66" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L66" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K66" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L66" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M66" s="3">
         <f t="shared" si="12"/>
@@ -5417,13 +5417,13 @@
         <v>2</v>
       </c>
       <c r="J67" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K67" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L67" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K67" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L67" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M67" s="3">
         <f t="shared" si="12"/>
@@ -5456,13 +5456,13 @@
         <v>2</v>
       </c>
       <c r="J68" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L68" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K68" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L68" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M68" s="3">
         <f t="shared" si="12"/>
@@ -5493,13 +5493,13 @@
         <v>2</v>
       </c>
       <c r="J69" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L69" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K69" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L69" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M69" s="3">
         <f t="shared" si="12"/>
@@ -5534,13 +5534,13 @@
         <v>2</v>
       </c>
       <c r="J70" s="3">
+        <f t="shared" si="11"/>
+      </c>
+      <c r="K70" s="3">
+        <f t="shared" si="13"/>
+      </c>
+      <c r="L70" s="3">
         <f t="shared" si="14"/>
-      </c>
-      <c r="K70" s="3">
-        <f t="shared" si="15"/>
-      </c>
-      <c r="L70" s="3">
-        <f t="shared" si="11"/>
       </c>
       <c r="M70" s="3">
         <f t="shared" si="12"/>
@@ -34645,214 +34645,214 @@
         <v>648</v>
       </c>
       <c r="C213" s="20">
-        <f ref="C213:BS213" t="shared" si="0">=SUM(C3:C211)</f>
+        <f ref="C213:BS213" t="shared" si="1">=SUM(C3:C211)</f>
       </c>
       <c r="D213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="E213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="F213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="G213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="H213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="I213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="J213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="K213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="L213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="M213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="N213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="O213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="P213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="Q213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="R213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="S213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="T213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="U213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="V213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="W213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="X213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="Y213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="Z213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AA213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AB213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AC213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AD213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AE213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AF213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AG213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AH213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AI213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AJ213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AK213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AL213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AM213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AN213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AO213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AP213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AQ213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AR213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AS213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AT213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AU213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AV213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AW213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AX213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AY213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="AZ213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BA213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BB213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BC213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BD213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BE213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BF213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BG213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BH213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BI213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BJ213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BK213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BL213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BM213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BN213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BO213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BP213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BQ213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BR213" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BS213" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="BT213" s="4">
-        <f ref="BT213:BT214" t="shared" si="1">=SUM(C213:BS213)</f>
+        <f ref="BT213:BT214" t="shared" si="0">=SUM(C213:BS213)</f>
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="true">
@@ -35070,7 +35070,7 @@
         <f>=IF(VLOOKUP(BS1,Potions!$A:$L,2)="common",4,IF(VLOOKUP(BS1,Potions!$A:$L,2)="uncommon",3,IF(VLOOKUP(BS1,Potions!$A:$L,2)="rare",5,IF(VLOOKUP(BS1,Potions!$A:$L,2)="very rare",7,9))))</f>
       </c>
       <c r="BT214" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="true">
@@ -35392,25 +35392,25 @@
         <f>=$C2*$N$2</f>
       </c>
       <c r="F2" s="2">
-        <f ref="F2:F6" t="shared" si="8">=E2*$N$3</f>
+        <f ref="F2:F6" t="shared" si="10">=E2*$N$3</f>
       </c>
       <c r="H2" s="2">
-        <f ref="H2:H6" t="shared" si="5">=G2*$N$4</f>
+        <f ref="H2:H6" t="shared" si="9">=G2*$N$4</f>
       </c>
       <c r="J2" s="2">
-        <f ref="J2:J6" t="shared" si="9">=I2*$N$5</f>
+        <f ref="J2:J6" t="shared" si="6">=I2*$N$5</f>
       </c>
       <c r="L2" s="2">
-        <f ref="L2:L6" t="shared" si="10">=K2*$N$6</f>
+        <f ref="L2:L6" t="shared" si="7">=K2*$N$6</f>
       </c>
       <c r="M2" s="4">
-        <f ref="M2:M6" t="shared" si="7">=C2+E2+G2+I2+K2</f>
+        <f ref="M2:M6" t="shared" si="8">=C2+E2+G2+I2+K2</f>
       </c>
       <c r="N2" s="2">
         <v>10</v>
       </c>
       <c r="O2" s="2">
-        <f ref="O2:O6" t="shared" si="6">=D2+F2+H2+J2+L2</f>
+        <f ref="O2:O6" t="shared" si="5">=D2+F2+H2+J2+L2</f>
       </c>
       <c r="P2" s="2">
         <v>50</v>
@@ -35436,25 +35436,25 @@
         <v>2</v>
       </c>
       <c r="F3" s="2">
+        <f t="shared" si="10"/>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="9"/>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="6"/>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" si="7"/>
+      </c>
+      <c r="M3" s="4">
         <f t="shared" si="8"/>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" si="5"/>
-      </c>
-      <c r="J3" s="2">
-        <f t="shared" si="9"/>
-      </c>
-      <c r="L3" s="2">
-        <f t="shared" si="10"/>
-      </c>
-      <c r="M3" s="4">
-        <f t="shared" si="7"/>
       </c>
       <c r="N3" s="2">
         <v>90</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
       </c>
       <c r="P3" s="2">
         <v>250</v>
@@ -35480,28 +35480,28 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
       </c>
       <c r="G4" s="2">
         <v>3</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
       </c>
       <c r="N4" s="2">
         <v>650</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
       </c>
       <c r="P4" s="2">
         <v>2500</v>
@@ -35524,31 +35524,31 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
       </c>
       <c r="G5" s="2">
         <v>4</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
       </c>
       <c r="I5" s="2">
         <v>2</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
       </c>
       <c r="N5" s="2">
         <v>8500</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
       </c>
       <c r="P5" s="2">
         <v>25000</v>
@@ -35571,34 +35571,34 @@
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
       </c>
       <c r="G6" s="2">
         <v>3</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
       </c>
       <c r="I6" s="2">
         <v>3</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
       </c>
       <c r="N6" s="2">
         <v>70000</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
       </c>
       <c r="P6" s="2">
         <v>125000</v>

</xml_diff>